<commit_message>
v0.47 Added Script, Fixed Register excel file, Fixed Sync, Dongle Inti and so on...
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_0.6.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_0.6.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="137">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -850,6 +850,10 @@
   </si>
   <si>
     <t>DOne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -996,7 +1000,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1036,6 +1040,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1078,7 +1083,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1122,7 +1127,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1166,7 +1171,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1902,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2164,7 +2169,7 @@
       </c>
     </row>
     <row r="34" spans="3:8" ht="24" customHeight="1">
-      <c r="E34" s="20">
+      <c r="E34" s="21">
         <v>2</v>
       </c>
       <c r="F34" s="10" t="s">
@@ -2172,7 +2177,7 @@
       </c>
     </row>
     <row r="35" spans="3:8" ht="108">
-      <c r="E35" s="20"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="11" t="s">
         <v>99</v>
       </c>
@@ -2195,6 +2200,9 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10" t="s">
         <v>63</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="3:8">

</xml_diff>